<commit_message>
Adding the bins works now
</commit_message>
<xml_diff>
--- a/src/main/resources/New_Bin_1.xlsx
+++ b/src/main/resources/New_Bin_1.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11100" yWindow="440" windowWidth="12040" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="hg">Feuil1!$I$4</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -27,14 +30,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="36">
   <si>
     <t>CFG</t>
   </si>
   <si>
-    <t>test_Automated_newBin</t>
-  </si>
-  <si>
     <t>Actif</t>
   </si>
   <si>
@@ -50,10 +50,94 @@
     <t>CFG CVK KEY</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>test_Automation_mags</t>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Jour</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>SVI</t>
+  </si>
+  <si>
+    <t>Inactif</t>
+  </si>
+  <si>
+    <t>MasterCard</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>SMPP</t>
+  </si>
+  <si>
+    <t>SMS</t>
+  </si>
+  <si>
+    <t>Service Web SMS</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Semaine</t>
+  </si>
+  <si>
+    <t>kepler</t>
+  </si>
+  <si>
+    <t>S2M</t>
+  </si>
+  <si>
+    <t>Mobile-Token</t>
+  </si>
+  <si>
+    <t>Anas</t>
+  </si>
+  <si>
+    <t>test_Automated_newBin_1</t>
+  </si>
+  <si>
+    <t>test_Automated_newBin_2</t>
+  </si>
+  <si>
+    <t>test_Automated_newBin_3</t>
+  </si>
+  <si>
+    <t>test_Automated_newBin_4</t>
+  </si>
+  <si>
+    <t>test_Automated_newBin_5</t>
+  </si>
+  <si>
+    <t>test_Automated_newBin_6</t>
+  </si>
+  <si>
+    <t>test_Automation_11</t>
+  </si>
+  <si>
+    <t>test_Automation_12</t>
+  </si>
+  <si>
+    <t>test_Automation_13</t>
+  </si>
+  <si>
+    <t>test_Automation_14</t>
+  </si>
+  <si>
+    <t>test_Automation_15</t>
+  </si>
+  <si>
+    <t>test_Automation_16</t>
+  </si>
+  <si>
+    <t>TEAM</t>
   </si>
 </sst>
 </file>
@@ -375,74 +459,459 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" customWidth="1"/>
     <col min="11" max="11" width="20.33203125" customWidth="1"/>
     <col min="12" max="12" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1">
+        <v>6</v>
+      </c>
+      <c r="E1">
+        <v>464000</v>
+      </c>
+      <c r="F1">
+        <v>464000</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="D1">
-        <v>6</v>
-      </c>
-      <c r="E1">
-        <v>464056</v>
-      </c>
-      <c r="F1">
-        <v>464056</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1">
+        <v>6</v>
+      </c>
+      <c r="P1">
+        <v>1000</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>464001</v>
+      </c>
+      <c r="F2">
+        <v>464001</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2">
+        <v>6</v>
+      </c>
+      <c r="P2">
+        <v>1000</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2">
+        <v>3000</v>
+      </c>
+      <c r="T2">
+        <v>1000</v>
+      </c>
+      <c r="U2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>464005</v>
+      </c>
+      <c r="F3">
+        <v>464005</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3">
+        <v>6</v>
+      </c>
+      <c r="P3">
+        <v>1000</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S3">
+        <v>3000</v>
+      </c>
+      <c r="T3">
+        <v>1000</v>
+      </c>
+      <c r="U3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>464003</v>
+      </c>
+      <c r="F4">
+        <v>464003</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4">
+        <v>6</v>
+      </c>
+      <c r="P4">
+        <v>1000</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" t="s">
+        <v>8</v>
+      </c>
+      <c r="U4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>464004</v>
+      </c>
+      <c r="F5">
+        <v>464004</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K5" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="L5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
         <v>7</v>
       </c>
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>9</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <v>11</v>
+      </c>
+      <c r="M8">
+        <v>12</v>
+      </c>
+      <c r="N8">
+        <v>13</v>
+      </c>
+      <c r="O8">
+        <v>14</v>
+      </c>
+      <c r="P8">
+        <v>15</v>
+      </c>
+      <c r="Q8">
+        <v>16</v>
+      </c>
+      <c r="R8">
+        <v>17</v>
+      </c>
+      <c r="S8">
+        <v>18</v>
+      </c>
+      <c r="T8">
+        <v>19</v>
+      </c>
+      <c r="U8">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>464002</v>
+      </c>
+      <c r="F12">
+        <v>464002</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N12" t="s">
+        <v>8</v>
+      </c>
+      <c r="O12" t="s">
+        <v>8</v>
+      </c>
+      <c r="P12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>9</v>
+      </c>
+      <c r="R12" t="s">
+        <v>7</v>
+      </c>
+      <c r="S12">
+        <v>200</v>
+      </c>
+      <c r="T12">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="U17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>